<commit_message>
Add Updated Data Log From Smell Test
</commit_message>
<xml_diff>
--- a/Data/data_log_from_smell_test.xlsx
+++ b/Data/data_log_from_smell_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/353caa7d06450a03/Documents/Projects/Smart Milk Spoilage Detection Experiment Data Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/353caa7d06450a03/Documents/Projects/Smart Milk Spoilage Detection Experiment Data Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="11_F25DC773A252ABDACC1048A431187B8C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{142D902A-617A-44C4-B9C5-548439B93D38}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="11_F25DC773A252ABDACC1048A431187B8C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96D1275C-AAF7-4C88-B478-ABF92A15ADD8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Timestamp</t>
   </si>
@@ -91,6 +91,45 @@
   </si>
   <si>
     <t>Temprature of the Unrefrigerated Milk Room (F)</t>
+  </si>
+  <si>
+    <t>12-06-2024 08:46AM</t>
+  </si>
+  <si>
+    <t>12-06-2024 09:55PM</t>
+  </si>
+  <si>
+    <t>12-07-2024 09:22AM</t>
+  </si>
+  <si>
+    <t>12-07-2024 08:05PM</t>
+  </si>
+  <si>
+    <t>12-08-2024 09:31AM</t>
+  </si>
+  <si>
+    <t>12-08-2024 07:12AM</t>
+  </si>
+  <si>
+    <t>12-09-2024 06:20AM</t>
+  </si>
+  <si>
+    <t>12-10-2024 06:18AM</t>
+  </si>
+  <si>
+    <t>12-10-2024 06:20PM</t>
+  </si>
+  <si>
+    <t>12-09-2024 09:07PM</t>
+  </si>
+  <si>
+    <t>12-11-2024 06:17AM</t>
+  </si>
+  <si>
+    <t>12-11-2024 08:55PM</t>
+  </si>
+  <si>
+    <t>12-12-2024 10:46AM</t>
   </si>
 </sst>
 </file>
@@ -414,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,6 +663,149 @@
         <v>7</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>38.5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>38.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>37.5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>38.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>38.5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>